<commit_message>
Add new front-end design
</commit_message>
<xml_diff>
--- a/req.xlsx
+++ b/req.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\101114992\Documents\Research\98Coding\00coderepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE118CDC-3DAC-4649-B4AA-8701CC7BEE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18810C6D-C734-41A0-8DE5-F89D636A2C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34035" yWindow="630" windowWidth="19335" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="3015" windowWidth="12840" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -61,13 +61,10 @@
     <t>crushedstone</t>
   </si>
   <si>
-    <t>Ojo</t>
-  </si>
-  <si>
     <t>lime</t>
   </si>
   <si>
-    <t>carbonate</t>
+    <t>Rock</t>
   </si>
 </sst>
 </file>
@@ -454,7 +451,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,94 +484,94 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>40</v>
       </c>
       <c r="F2" s="1">
-        <v>44662</v>
+        <v>44665</v>
       </c>
       <c r="G2" s="2">
-        <v>0.54167824074074067</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>34</v>
       </c>
       <c r="F3" s="1">
-        <v>44662</v>
+        <v>44665</v>
       </c>
       <c r="G3" s="2">
-        <v>0.5417939814814815</v>
+        <v>0.41679398148148145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>60</v>
       </c>
       <c r="F4" s="1">
-        <v>44662</v>
+        <v>44665</v>
       </c>
       <c r="G4" s="2">
-        <v>0.54190972222222222</v>
+        <v>0.41689814814814818</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>28</v>
       </c>
       <c r="F5" s="1">
-        <v>44662</v>
+        <v>44665</v>
       </c>
       <c r="G5" s="2">
-        <v>0.54207175925925932</v>
+        <v>0.41724537037037041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>